<commit_message>
new java file added in ruf package
</commit_message>
<xml_diff>
--- a/testdata/testData.xlsx
+++ b/testdata/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frameworks\Selenium_Training_Code\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frameworks\POMFramework\Selenium_Training_Code\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Locator</t>
   </si>
@@ -49,6 +49,21 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>MyWishList1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First WishList </t>
+  </si>
+  <si>
+    <t>MyWishList2</t>
+  </si>
+  <si>
+    <t>Second Wishlist</t>
+  </si>
+  <si>
+    <t>Third Wishlist</t>
   </si>
 </sst>
 </file>
@@ -375,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,6 +424,30 @@
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New files updated on 3/01/2017
</commit_message>
<xml_diff>
--- a/testdata/testData.xlsx
+++ b/testdata/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frameworks\Selenium_Training_Code\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frameworks\POMFramework\Selenium_Training_Code\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Locator</t>
   </si>
@@ -49,6 +49,24 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>MyWishList1</t>
+  </si>
+  <si>
+    <t>New WishList1</t>
+  </si>
+  <si>
+    <t>MyWishList2</t>
+  </si>
+  <si>
+    <t>New WishList2</t>
+  </si>
+  <si>
+    <t>MyWishList3</t>
+  </si>
+  <si>
+    <t>New WishList3</t>
   </si>
 </sst>
 </file>
@@ -375,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,6 +427,30 @@
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>